<commit_message>
docs(pipelining): add testing program with more structural hazards
</commit_message>
<xml_diff>
--- a/programs/movsshiftinginstructions.xlsx
+++ b/programs/movsshiftinginstructions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vacla\Projects\cpu\programs\pipelining\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vacla\Projects\cpu\programs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E61B2A35-1774-4140-B38F-B0ACB4039CEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C948B97-38BA-4D24-948D-372A006455FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E410B2C1-F054-41C4-A96D-F1120FBD95E0}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{E410B2C1-F054-41C4-A96D-F1120FBD95E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Code" sheetId="1" r:id="rId1"/>
@@ -568,7 +568,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8E17FB6-AC76-4C3E-BEFA-6AB3607784FD}">
   <dimension ref="A1:U29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="U11" sqref="U11"/>
     </sheetView>
   </sheetViews>
@@ -1195,6 +1195,16 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="M4:P4"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="D5:H5"/>
+    <mergeCell ref="I5:R5"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="K6:P6"/>
     <mergeCell ref="D2:F2"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="K2:M2"/>
@@ -1204,16 +1214,6 @@
     <mergeCell ref="K3:N3"/>
     <mergeCell ref="O3:P3"/>
     <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="K6:P6"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="M4:P4"/>
-    <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="D5:H5"/>
-    <mergeCell ref="I5:R5"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1225,8 +1225,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41F3C705-99AD-4EB4-93AB-8ACC410281DE}">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>